<commit_message>
EPBDS-8800 Error in table with empty merged cells in return
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/sheet-optimization.xlsx
+++ b/DEV/org.openl.rules/test/rules/sheet-optimization.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\openl\DEV\org.openl.rules\test\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692BBD70-CBA0-4B19-9B15-7A6644CE6F6B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C740F6F8-86B4-48B2-8BF1-B86608B6C015}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B6DF97B9-5A3C-4A78-92F7-D430747C6C35}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B6DF97B9-5A3C-4A78-92F7-D430747C6C35}"/>
   </bookViews>
   <sheets>
     <sheet name="Wider merged cells" sheetId="2" r:id="rId1"/>
     <sheet name="Empty merged cells" sheetId="3" r:id="rId2"/>
+    <sheet name="Merged cells can't be deleted" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -333,7 +334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>money</t>
   </si>
@@ -437,16 +438,130 @@
       <t xml:space="preserve"> (Expense expense)</t>
     </r>
   </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>HC1</t>
+  </si>
+  <si>
+    <t>HC2</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>referenceName</t>
+  </si>
+  <si>
+    <t>attributeName</t>
+  </si>
+  <si>
+    <t>new Double[] {min,max, step}</t>
+  </si>
+  <si>
+    <t>Double min</t>
+  </si>
+  <si>
+    <t>Double max</t>
+  </si>
+  <si>
+    <t>Double step</t>
+  </si>
+  <si>
+    <t>Comp Ref Name</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>GOLD</t>
+  </si>
+  <si>
+    <t>SILVER</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules Double[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+      </rPr>
+      <t>testLookup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> ( ReferenceName referenceName, AttributeName attributeName, Dimension dimension )</t>
+    </r>
+  </si>
+  <si>
+    <t>Ref2</t>
+  </si>
+  <si>
+    <t>Ref3</t>
+  </si>
+  <si>
+    <t>dimField1</t>
+  </si>
+  <si>
+    <t>dimField2</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>Ref1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="11">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="172" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="173" formatCode="_ * #,##0.00_)\ _$_ ;_ * \(#,##0.00\)\ _$_ ;_ * &quot;-&quot;??_)\ _$_ ;_ @_ "/>
+    <numFmt numFmtId="174" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="175" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,8 +704,185 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="186"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="9" tint="-0.24994659260841701"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="186"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color theme="1"/>
+      <name val="verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,8 +930,114 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="61">
     <border>
       <left/>
       <right/>
@@ -911,14 +1309,737 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="5" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="25" fillId="4" borderId="31" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="25" fillId="5" borderId="17">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="32" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="172" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="174" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="174" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="174" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="174" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="175" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="43" fillId="9" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1029,6 +2150,9 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1053,26 +2177,424 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="28" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="29" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="38" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="39" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="38" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="40" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="41" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="40" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="36" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="37" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="49" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="50" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="49" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="2" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="4" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="54" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="4" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="54" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="36" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="51" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="37" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="29" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="58" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="8" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="30" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="59" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="28" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="56" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="60" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="57" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="55" xfId="248" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="42" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="43" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="44" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="42" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="43" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="44" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="46" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="45" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="47" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="48" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="45" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="52" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="53" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="249">
+    <cellStyle name="20% - Accent1 2" xfId="7" xr:uid="{A72B5921-BD82-4599-8C2E-9D53B57768F3}"/>
+    <cellStyle name="20% - Accent1 3" xfId="8" xr:uid="{C707F783-61BF-47C8-BC42-6621C9FE78D6}"/>
+    <cellStyle name="20% - Accent1 4" xfId="9" xr:uid="{773BD52C-6E97-4273-9573-BEF8F69AD9DD}"/>
+    <cellStyle name="20% - Accent1 5" xfId="10" xr:uid="{E2BC1AEB-46E2-4E31-AA9E-3B3503FBDEC1}"/>
+    <cellStyle name="20% - Accent1 5 2" xfId="11" xr:uid="{CFA0E5BB-051E-4469-BABB-3D279496695C}"/>
+    <cellStyle name="20% - Accent1 5 2 2" xfId="12" xr:uid="{BE78160D-9523-44EB-B73E-B5058D5C03B5}"/>
+    <cellStyle name="20% - Accent1 5 2 2 2" xfId="13" xr:uid="{867D6E30-7057-4945-93F5-B7205674E4BC}"/>
+    <cellStyle name="20% - Accent1 5 2 2_DBASE" xfId="14" xr:uid="{CDD20C75-4051-4B25-8A2D-1CD665F65E5C}"/>
+    <cellStyle name="20% - Accent1 5 2 3" xfId="15" xr:uid="{B2363856-DD38-48E0-BB78-47E108AF1751}"/>
+    <cellStyle name="20% - Accent1 5 2_DBASE" xfId="16" xr:uid="{E68EF4E6-CC4F-4901-8313-5D1DEC5DC197}"/>
+    <cellStyle name="20% - Accent1 5 3" xfId="17" xr:uid="{ABF64706-AE00-4E4A-984D-E37E1E1FEDB3}"/>
+    <cellStyle name="20% - Accent1 5 3 2" xfId="18" xr:uid="{188A9F0E-70A9-4452-B846-B14ED8FB7CB7}"/>
+    <cellStyle name="20% - Accent1 5 3_DBASE" xfId="19" xr:uid="{2203C1D9-BFDD-4447-AD23-4474545622EB}"/>
+    <cellStyle name="20% - Accent1 5 4" xfId="20" xr:uid="{27764EB6-E219-40AB-9A61-E8B7F7C70F48}"/>
+    <cellStyle name="20% - Accent1 5_DBASE" xfId="21" xr:uid="{B6B66F20-6CEE-4509-8134-CDA84AD79A4F}"/>
+    <cellStyle name="20% - Accent1 6" xfId="22" xr:uid="{47D69D7A-941B-4B5E-8285-2D39612A3560}"/>
+    <cellStyle name="20% - Accent1 6 2" xfId="23" xr:uid="{DEAA8C13-F029-4146-BB30-5D2656BEBFFE}"/>
+    <cellStyle name="20% - Accent1 6_DBASE" xfId="24" xr:uid="{FACC986B-F93F-4624-9848-DEE487F1A156}"/>
+    <cellStyle name="20% - Accent1 7" xfId="25" xr:uid="{CC05E7C7-EFC0-405E-90B6-51EF7352DD51}"/>
+    <cellStyle name="20% - Accent1 8" xfId="26" xr:uid="{038E5E0F-3B36-4DA2-8CE5-B8F22C5A0B34}"/>
+    <cellStyle name="20% - Accent2 2" xfId="27" xr:uid="{BF2C31BD-382C-429E-B185-ACE202F66310}"/>
+    <cellStyle name="20% - Accent2 3" xfId="28" xr:uid="{6D06EDEB-4DC5-4F40-96C9-D95F978B4F53}"/>
+    <cellStyle name="20% - Accent2 4" xfId="29" xr:uid="{CB470506-ECC3-4B29-BC90-122BB607A61B}"/>
+    <cellStyle name="20% - Accent3 2" xfId="30" xr:uid="{62A88318-9005-4B8D-8392-8E403701DD47}"/>
+    <cellStyle name="20% - Accent3 3" xfId="31" xr:uid="{10A00828-A530-4D2C-9D6F-AD7AB5D46732}"/>
+    <cellStyle name="20% - Accent3 4" xfId="32" xr:uid="{224491AC-1140-4445-9DF6-447453D37177}"/>
+    <cellStyle name="20% - Accent4 2" xfId="33" xr:uid="{FF6F1287-360C-48DC-81D2-96CD22AC3B5E}"/>
+    <cellStyle name="20% - Accent4 3" xfId="34" xr:uid="{1C2B5231-352F-4549-B8B9-07134B8C5E58}"/>
+    <cellStyle name="20% - Accent4 4" xfId="35" xr:uid="{83FEA334-8564-455C-B7D3-E095BA5C2740}"/>
+    <cellStyle name="20% - Accent5 2" xfId="36" xr:uid="{EB85FAF4-89F4-4819-9245-67F12641A227}"/>
+    <cellStyle name="20% - Accent5 3" xfId="37" xr:uid="{69B3ABFD-2672-4D1D-A58F-1E856BA72A55}"/>
+    <cellStyle name="20% - Accent5 4" xfId="38" xr:uid="{33BD9F09-1943-45A4-9FA6-E1280B9DC48F}"/>
+    <cellStyle name="20% - Accent6 2" xfId="39" xr:uid="{82C75FD3-B48B-45EB-8D4F-FEE14FD760F5}"/>
+    <cellStyle name="20% - Accent6 2 2" xfId="40" xr:uid="{DCFB3108-20EF-4F84-B7A5-F5577BF14FAD}"/>
+    <cellStyle name="20% - Accent6 3" xfId="41" xr:uid="{C62787BE-FFDC-4EC6-9F20-9F2E74DFFE94}"/>
+    <cellStyle name="20% - Accent6 4" xfId="42" xr:uid="{98A39D4A-A47D-4287-82AC-9E87C0268E04}"/>
+    <cellStyle name="40% - Accent1 2" xfId="43" xr:uid="{68C83F5A-52FB-4010-9C73-A6DA6DADCA10}"/>
+    <cellStyle name="40% - Accent1 3" xfId="44" xr:uid="{DA1340ED-E583-4B09-9D94-76657FB5195D}"/>
+    <cellStyle name="40% - Accent1 4" xfId="45" xr:uid="{E7023C80-944F-449F-9CCF-6AF7E85DFE35}"/>
+    <cellStyle name="40% - Accent2 2" xfId="46" xr:uid="{B2D02225-7DCB-4276-BDF1-CD53BFC9B499}"/>
+    <cellStyle name="40% - Accent2 3" xfId="47" xr:uid="{74D6861B-C95C-4109-8F7C-AC95E610738C}"/>
+    <cellStyle name="40% - Accent2 4" xfId="48" xr:uid="{522A36CE-B8BD-4603-8494-CA9C3AD2437F}"/>
+    <cellStyle name="40% - Accent3 2" xfId="49" xr:uid="{ABB5B9C5-97A3-4E87-96AB-7ADA47DA026E}"/>
+    <cellStyle name="40% - Accent3 3" xfId="50" xr:uid="{007A9FCA-D642-4320-A105-38B9E1992199}"/>
+    <cellStyle name="40% - Accent3 4" xfId="51" xr:uid="{DB0736A0-C6C2-4304-AFC8-A97E6D3A19CF}"/>
+    <cellStyle name="40% - Accent4 2" xfId="52" xr:uid="{EDA23CB5-880B-4526-A354-68AE3F5DEAEE}"/>
+    <cellStyle name="40% - Accent4 3" xfId="53" xr:uid="{AE2F2BBB-63FB-4EA0-8273-99B4D4D756AB}"/>
+    <cellStyle name="40% - Accent4 4" xfId="54" xr:uid="{64C2A8F1-4F8F-4CC5-9725-8CB48A1C4B1F}"/>
+    <cellStyle name="40% - Accent5 2" xfId="55" xr:uid="{3F5C5924-7EF2-4EE3-97D9-059F11AECF67}"/>
+    <cellStyle name="40% - Accent5 3" xfId="56" xr:uid="{93DC9B35-B546-4CD6-8373-72BFB35803E5}"/>
+    <cellStyle name="40% - Accent5 4" xfId="57" xr:uid="{B86471B8-F418-4972-AC56-642A36FA0858}"/>
+    <cellStyle name="40% - Accent6 2" xfId="58" xr:uid="{1DF4063C-F472-4DCC-80A9-1E121121027A}"/>
+    <cellStyle name="40% - Accent6 3" xfId="59" xr:uid="{D32F1078-FACF-4DB0-99DE-25279ACFE74E}"/>
+    <cellStyle name="40% - Accent6 4" xfId="60" xr:uid="{A0B2A0F3-54E5-4A2C-931F-259D550EB496}"/>
+    <cellStyle name="ACT_B" xfId="61" xr:uid="{0B09567C-3F56-4DA6-8B35-6F3FE7F9E9B5}"/>
+    <cellStyle name="CD" xfId="62" xr:uid="{EC299825-3C83-4D37-92CA-A28F8504F26F}"/>
+    <cellStyle name="Comma 2" xfId="63" xr:uid="{AFB158B7-051C-4010-AD11-EF7805327A29}"/>
+    <cellStyle name="Comma 2 2" xfId="64" xr:uid="{446CEB5E-A774-40D7-8479-FC36AC7B4A4D}"/>
+    <cellStyle name="Comma 2 2 2" xfId="65" xr:uid="{70A248A5-3C59-463A-839E-BF7F151C2E7C}"/>
+    <cellStyle name="Comma 2 2 3" xfId="66" xr:uid="{1FA89407-CAB0-4962-AECA-CACAA3BF1BB2}"/>
+    <cellStyle name="Comma 2 3" xfId="67" xr:uid="{1B9DD5F2-DCA2-4DFE-90AF-EA69A3B397E1}"/>
+    <cellStyle name="Comma 2 3 2" xfId="68" xr:uid="{1FAD047E-4873-46DB-A239-BD0DC3878873}"/>
+    <cellStyle name="Comma 2 4" xfId="69" xr:uid="{05A55F35-E75A-4D80-AE7A-290D8A0790BB}"/>
+    <cellStyle name="Comma 2 5" xfId="70" xr:uid="{76FC1C7F-A8DB-41AF-BA16-4E7AD7E60648}"/>
+    <cellStyle name="Comma 2 5 2" xfId="71" xr:uid="{9E872427-F96B-4621-97A6-D1AF2D71A661}"/>
+    <cellStyle name="Comma 2 6" xfId="72" xr:uid="{5736F53B-02EE-4FD7-9130-364E686CA011}"/>
+    <cellStyle name="Comma 3" xfId="73" xr:uid="{61C52E2F-2D3B-46CD-9DD1-4900E5AB28CA}"/>
+    <cellStyle name="Comma 3 2" xfId="74" xr:uid="{AC35B6F2-F248-4C36-A40C-FD1220E5FA19}"/>
+    <cellStyle name="Comma 3 3" xfId="75" xr:uid="{5648C4E0-CAD8-41F4-97C1-D93F41BD9AEA}"/>
+    <cellStyle name="Comma 4" xfId="76" xr:uid="{93D7CE7F-A14A-4EC0-9500-5E5CA4FE72C6}"/>
+    <cellStyle name="Comma 5" xfId="77" xr:uid="{F5ABB22C-2BBB-4814-A3C9-DB2764E09D94}"/>
+    <cellStyle name="Comment" xfId="78" xr:uid="{A5685DC5-F129-49B8-A514-DF7A4E00D3CA}"/>
+    <cellStyle name="COND_B" xfId="79" xr:uid="{AC404392-0597-4E53-828F-B5F6F5181BE4}"/>
+    <cellStyle name="Currency 2" xfId="80" xr:uid="{5A559609-CA68-4D34-8F38-C121F6454C68}"/>
+    <cellStyle name="Currency 2 2" xfId="81" xr:uid="{6EB1C3A0-E2C7-4F57-A38D-935BAFF34165}"/>
+    <cellStyle name="Currency 2 2 2" xfId="82" xr:uid="{1C511B8F-8B1C-4C41-997C-81A16CB3CDBA}"/>
+    <cellStyle name="Currency 2 3" xfId="83" xr:uid="{812500F6-496E-436A-993D-9CC914803132}"/>
+    <cellStyle name="Currency 2 4" xfId="84" xr:uid="{88BB2DC6-BF39-46B0-97E6-C6EB86F6A202}"/>
+    <cellStyle name="Currency 2 4 2" xfId="85" xr:uid="{B0B8AF7E-4784-444F-8EE5-531EFE69A324}"/>
+    <cellStyle name="Currency 2 5" xfId="86" xr:uid="{11696AAB-B58D-4FC8-B4CC-1092BF742D55}"/>
+    <cellStyle name="Currency 3" xfId="87" xr:uid="{35DE63E0-15DA-4955-9F04-8BC0E3848695}"/>
+    <cellStyle name="Currency 3 2" xfId="88" xr:uid="{677A2142-420F-458F-99CC-6F712BCDF4DD}"/>
+    <cellStyle name="Currency 3 3" xfId="89" xr:uid="{23C3E90F-D0DB-484C-A8E0-3D045F4E71D9}"/>
+    <cellStyle name="Currency 4" xfId="90" xr:uid="{C96AB606-C38F-4AF2-A842-A85C1996D90E}"/>
+    <cellStyle name="Currency 5" xfId="91" xr:uid="{854B0AB7-65B2-4F47-94CC-7D53A52786AA}"/>
+    <cellStyle name="Data type header" xfId="92" xr:uid="{D1C2A1BE-A3D0-41DF-B0EC-F7A9E33CF715}"/>
+    <cellStyle name="Data type header 2" xfId="93" xr:uid="{C155F6CD-7F25-46FA-BE12-123DA1EF8C14}"/>
+    <cellStyle name="Data type header 2 2" xfId="94" xr:uid="{2811CF93-3BC5-46CE-8409-E0B731AB1CC7}"/>
+    <cellStyle name="Data type header 2 2 2" xfId="95" xr:uid="{89296269-4FC4-44CE-8D17-2C06A5691E33}"/>
+    <cellStyle name="Data type header 2 2 2 2" xfId="96" xr:uid="{34561E11-5588-4F61-82F2-18F574C7ADEF}"/>
+    <cellStyle name="Data type header 2 2 3" xfId="97" xr:uid="{75DC643B-7F34-44CE-A662-AC94F6D255A1}"/>
+    <cellStyle name="Data type header 2 2_DBASE" xfId="98" xr:uid="{C12B9F9B-43BD-45CE-B088-52ECFA6F285C}"/>
+    <cellStyle name="Data type header 2 3" xfId="99" xr:uid="{A342E77D-8AAF-41B5-B17C-A2BA96DE0FD1}"/>
+    <cellStyle name="Data type header 2 3 2" xfId="100" xr:uid="{D49DFEAF-BCD5-40C0-9DD5-0F8E94011FC4}"/>
+    <cellStyle name="Data type header 2 4" xfId="101" xr:uid="{5126F689-9B20-4698-9E55-3B0745060C84}"/>
+    <cellStyle name="Data type header 2_DBASE" xfId="102" xr:uid="{181E0C81-D8C3-42DF-AB5D-4E1A4FC257D7}"/>
+    <cellStyle name="Data type header 3" xfId="103" xr:uid="{40C0C4AE-948C-475A-A623-1F3052DF73D3}"/>
+    <cellStyle name="Data type header 3 2" xfId="104" xr:uid="{EA09A62F-F7DA-4F5B-90BA-E1C9181CAC21}"/>
+    <cellStyle name="Data type header 3 2 2" xfId="105" xr:uid="{9A7FBDA9-E8C7-431A-BFA2-74F486E2C401}"/>
+    <cellStyle name="Data type header 3 3" xfId="106" xr:uid="{C845B1D4-B52B-43FE-AC9C-F2F82E32FF8A}"/>
+    <cellStyle name="Data type header 3_DBASE" xfId="107" xr:uid="{F2A4EB24-2D28-4DF4-8942-E697632FE4F4}"/>
+    <cellStyle name="Data type header 4" xfId="108" xr:uid="{C9B6B1B8-EF64-4A23-8FDD-DA2EF3A9BE5C}"/>
+    <cellStyle name="Data type header 4 2" xfId="109" xr:uid="{B417C40F-CBDE-4374-9AF2-FBDD95F57578}"/>
+    <cellStyle name="Data type header 5" xfId="110" xr:uid="{5BACF845-2FE3-4566-BD69-387F523B9165}"/>
+    <cellStyle name="Data type header_DBASE" xfId="111" xr:uid="{42CFF1AA-F3AD-4AD3-9B76-C07C26849E2A}"/>
+    <cellStyle name="Datatype" xfId="112" xr:uid="{4D19DAEF-D548-4917-ACF3-FC7C9F52E21E}"/>
+    <cellStyle name="Euro" xfId="113" xr:uid="{947E1609-BEA4-4B8E-A2BA-35DB3570F8F8}"/>
+    <cellStyle name="Euro 2" xfId="114" xr:uid="{D55D36C9-0831-47E8-AF60-68756114FD7B}"/>
+    <cellStyle name="H1" xfId="115" xr:uid="{221E3505-7595-4383-BB71-685C152FFAF5}"/>
+    <cellStyle name="H1 2" xfId="116" xr:uid="{06B74781-062C-4E5A-88F4-DF3E62D61D44}"/>
+    <cellStyle name="H2" xfId="117" xr:uid="{7C144B56-B03D-48BF-BE4C-9548E380DDD0}"/>
+    <cellStyle name="Heading 1 2" xfId="118" xr:uid="{C12F12E0-441F-4D4D-9034-5ACD797323BB}"/>
+    <cellStyle name="Heading 2 2" xfId="119" xr:uid="{CFE7C775-5CEC-478B-A228-573F985ADE88}"/>
+    <cellStyle name="Hyperlink 2" xfId="120" xr:uid="{A9C576C0-1797-40F0-8C7D-1B7423EB7F69}"/>
+    <cellStyle name="Hyperlink 3" xfId="121" xr:uid="{487772B0-406D-4B9A-B013-0FD7E8E86389}"/>
+    <cellStyle name="Input 2" xfId="241" xr:uid="{8DFAA780-8966-4147-ACB8-2DF4F199B430}"/>
+    <cellStyle name="Lien hypertexte 2" xfId="222" xr:uid="{2F7E34A4-3671-4A7F-9660-A60C66DE08FA}"/>
+    <cellStyle name="Lien hypertexte 2 2" xfId="223" xr:uid="{3A1E82C2-78C2-4DC6-984A-3F47D8946376}"/>
+    <cellStyle name="Milliers 2" xfId="224" xr:uid="{BEC726D4-9740-4427-9F07-F3891DD5F258}"/>
+    <cellStyle name="Milliers 2 2" xfId="225" xr:uid="{74E06BEB-77BC-45B4-8AF7-9D1978203317}"/>
+    <cellStyle name="Milliers 2 2 2" xfId="226" xr:uid="{394F7CF8-99DF-4EA6-8C00-5C5E121AC7D0}"/>
+    <cellStyle name="Milliers 2 3" xfId="227" xr:uid="{C5833F77-077C-454F-87B3-9E12DCB26470}"/>
+    <cellStyle name="Milliers 3" xfId="228" xr:uid="{0AECDAE1-9CB7-4CD3-BAA1-F354AF5E0075}"/>
+    <cellStyle name="Milliers 3 2" xfId="229" xr:uid="{0A1524F3-2159-41E3-AF98-AE71312C9C5F}"/>
+    <cellStyle name="Monétaire 2" xfId="230" xr:uid="{BFC6ECE9-A47C-404B-9339-6338A0837DD9}"/>
+    <cellStyle name="Monétaire 2 2" xfId="231" xr:uid="{486A7186-8174-4DB1-982E-B56D3AAF15FD}"/>
+    <cellStyle name="Monétaire 3" xfId="232" xr:uid="{0946F905-E158-4A95-BDB9-DC8471DE68C3}"/>
+    <cellStyle name="Monétaire 3 2" xfId="233" xr:uid="{53636741-F355-413E-9639-1AE95332935A}"/>
+    <cellStyle name="Normal 10" xfId="122" xr:uid="{3B8AC33C-8A5B-4912-9F7F-0A29F653FF73}"/>
+    <cellStyle name="Normal 10 2" xfId="123" xr:uid="{F37EDC45-7A9C-4B83-81D5-FAA161713A55}"/>
+    <cellStyle name="Normal 10 2 2" xfId="124" xr:uid="{BC0666D1-8471-4C16-920B-28ACA4B21CC8}"/>
+    <cellStyle name="Normal 10 3" xfId="125" xr:uid="{EEE0ED7F-4AD0-4BC5-9E6B-E38DCB6727DB}"/>
+    <cellStyle name="Normal 10 5" xfId="234" xr:uid="{D2138793-8D42-46BE-8C41-1ABED1C6521B}"/>
+    <cellStyle name="Normal 10 5 2" xfId="235" xr:uid="{FD5633B6-FB38-45E2-AB51-91ED12961AB5}"/>
+    <cellStyle name="Normal 11" xfId="126" xr:uid="{793522B3-807E-45E6-82F7-B12653CE2868}"/>
+    <cellStyle name="Normal 11 2" xfId="127" xr:uid="{35E145CA-5E53-4446-A3D9-CA83BFC9E625}"/>
+    <cellStyle name="Normal 11 3" xfId="128" xr:uid="{CC063867-7F65-4A3D-AA57-99087C8C8CC0}"/>
+    <cellStyle name="Normal 12" xfId="129" xr:uid="{DFA861D3-EF7B-4666-8D51-3787950B2B56}"/>
+    <cellStyle name="Normal 12 2 2 2" xfId="236" xr:uid="{7ED1ECB3-E61D-42AB-A6C1-436356473C0B}"/>
+    <cellStyle name="Normal 12 2 2 2 2" xfId="221" xr:uid="{A69B77DB-226D-4B31-BE6D-F7C6386C96D8}"/>
+    <cellStyle name="Normal 13" xfId="130" xr:uid="{8D856A0B-89C6-4631-8007-B308B5F8E673}"/>
+    <cellStyle name="Normal 13 13 2 2 2 2" xfId="131" xr:uid="{15D942EA-34DA-47FA-A422-927D04C08A15}"/>
+    <cellStyle name="Normal 13 2" xfId="237" xr:uid="{DAB44ECC-688F-4214-B4DD-CF893D5159BF}"/>
+    <cellStyle name="Normal 14" xfId="132" xr:uid="{A81409AB-0457-4408-A0C0-351EB1CACFA4}"/>
+    <cellStyle name="Normal 15" xfId="133" xr:uid="{8AB41FA3-2E55-4FCB-9507-DCC045B8E3E6}"/>
+    <cellStyle name="Normal 15 2" xfId="134" xr:uid="{A9636609-D756-4E7A-8B1D-71E3227FB448}"/>
+    <cellStyle name="Normal 16" xfId="135" xr:uid="{6D22AE58-1DAC-4868-BB3D-C92A74519526}"/>
+    <cellStyle name="Normal 16 2" xfId="136" xr:uid="{B3DA10E0-1712-4475-A355-6D646261A67A}"/>
+    <cellStyle name="Normal 17" xfId="240" xr:uid="{7CD26DE2-047D-4124-BC06-4A6A4BC73587}"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{2375932F-5832-4ABE-A4A7-BB37C4F6CC34}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{27BA8D7F-BE1D-41BE-AF6E-4675A0E1B37C}"/>
+    <cellStyle name="Normal 2 2 2" xfId="138" xr:uid="{B4AAB1FD-B650-4C93-B154-FD56A8D98B78}"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="139" xr:uid="{10F21EE9-6E9E-4FEE-B810-565F0AF8350D}"/>
+    <cellStyle name="Normal 2 2 2 3" xfId="140" xr:uid="{78E26020-D8EE-4060-B9D5-960EFFADFFBF}"/>
+    <cellStyle name="Normal 2 2 2 4" xfId="244" xr:uid="{0B42172B-1D93-4335-962E-1674044D2F6A}"/>
+    <cellStyle name="Normal 2 2 3" xfId="141" xr:uid="{6E7AFF7B-C9A1-4662-A0A8-26A182142BE7}"/>
+    <cellStyle name="Normal 2 2 4" xfId="142" xr:uid="{A88250A1-1CB0-42F2-B8D2-3A2E4E7518DF}"/>
+    <cellStyle name="Normal 2 2 5" xfId="243" xr:uid="{E822A2D4-A0BD-41AD-AEC9-DDF1F35CEAE2}"/>
+    <cellStyle name="Normal 2 3" xfId="143" xr:uid="{74A5E35B-4FF8-42F8-9F42-F91A75B0791A}"/>
+    <cellStyle name="Normal 2 3 2" xfId="144" xr:uid="{CDE6CC54-E819-4DB3-B948-9014912AE113}"/>
+    <cellStyle name="Normal 2 3 2 2" xfId="145" xr:uid="{A9788C2D-1FE1-4C2B-B3FF-07331BB78400}"/>
+    <cellStyle name="Normal 2 3 3" xfId="146" xr:uid="{A0DD1569-1E66-4F2E-9BBB-FE61C532D35B}"/>
+    <cellStyle name="Normal 2 3 4" xfId="147" xr:uid="{9131A81A-0A83-4696-9813-6CD2CDA43509}"/>
+    <cellStyle name="Normal 2 3 5" xfId="245" xr:uid="{05F49285-E7AC-46AC-A917-03FF1AE39C88}"/>
+    <cellStyle name="Normal 2 4" xfId="148" xr:uid="{D76A11D4-5C20-46A0-B7E0-CCB9DF2DDEE2}"/>
+    <cellStyle name="Normal 2 4 2" xfId="149" xr:uid="{9B72D49C-3D03-4F1B-98EC-290719E9B622}"/>
+    <cellStyle name="Normal 2 5" xfId="150" xr:uid="{E2616BFB-48D8-442B-8252-3183F7EC8834}"/>
+    <cellStyle name="Normal 2 5 2" xfId="151" xr:uid="{C41DB935-C093-44EF-BEC0-E6363366E9FC}"/>
+    <cellStyle name="Normal 2 5 3" xfId="152" xr:uid="{237208A3-63EA-4A05-A7F3-19FAE85C8164}"/>
+    <cellStyle name="Normal 2 6" xfId="242" xr:uid="{718FB5D2-EEFE-46E2-A582-86B0A32E8423}"/>
+    <cellStyle name="Normal 2 7" xfId="137" xr:uid="{1787E924-643E-4D11-A25D-E8E9F44D4E03}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{5933E63C-0C38-41F7-8C92-E306B1A634DD}"/>
+    <cellStyle name="Normal 3 2" xfId="153" xr:uid="{1E82B672-59BC-4CD7-A18F-91B9B7792489}"/>
+    <cellStyle name="Normal 3 2 2" xfId="154" xr:uid="{AEEF9933-3559-4821-895E-BDD7816FF806}"/>
+    <cellStyle name="Normal 3 2 3" xfId="155" xr:uid="{0C63A016-142F-4586-8D4A-C96EC15DF93B}"/>
+    <cellStyle name="Normal 3 2 4" xfId="246" xr:uid="{2F8981E1-796C-45B2-90BE-F08D646007D5}"/>
+    <cellStyle name="Normal 3 3" xfId="156" xr:uid="{547C78F4-99E1-41C8-ACE4-61C964E976C9}"/>
+    <cellStyle name="Normal 3 3 2" xfId="157" xr:uid="{99F4744A-362B-4C8B-8DB7-9AFA96634812}"/>
+    <cellStyle name="Normal 3 4" xfId="158" xr:uid="{4D6B1E97-28CE-44E2-9C4A-77D30383B6CC}"/>
+    <cellStyle name="Normal 3 4 2" xfId="159" xr:uid="{61D4B3E7-F72C-4FB7-AFD2-1A272802FDC8}"/>
+    <cellStyle name="Normal 4" xfId="160" xr:uid="{C7AE6EF3-A8B6-4343-9EF6-9EB656FBCDFB}"/>
+    <cellStyle name="Normal 4 2" xfId="161" xr:uid="{B698EC25-9574-4D0E-9B5C-5CF8A281B95C}"/>
+    <cellStyle name="Normal 4 2 2" xfId="162" xr:uid="{9D5D1666-8BF9-4E32-9824-A1F4E1331F02}"/>
+    <cellStyle name="Normal 4 3" xfId="163" xr:uid="{F8D677BA-4086-42A7-8CED-D39A41DC9772}"/>
+    <cellStyle name="Normal 4 3 2" xfId="164" xr:uid="{72E14096-4CCA-45C5-AD1B-AD7351FCBFC6}"/>
+    <cellStyle name="Normal 4 3 3" xfId="165" xr:uid="{3252D719-60DF-4723-A70E-95AE7237C943}"/>
+    <cellStyle name="Normal 4 4" xfId="166" xr:uid="{9762160A-6333-4F24-BB60-CC1835EDA33F}"/>
+    <cellStyle name="Normal 5" xfId="167" xr:uid="{76184CB2-7A78-440E-A437-A792CEACBFC3}"/>
+    <cellStyle name="Normal 5 2" xfId="168" xr:uid="{594C119C-79FC-46E5-A783-251AB1E83EFC}"/>
+    <cellStyle name="Normal 5 2 2" xfId="169" xr:uid="{CD2FF8BA-7F79-42C8-B933-6CDE12ED18DD}"/>
+    <cellStyle name="Normal 5 2 3" xfId="170" xr:uid="{ABF5CFB9-A118-42F2-B689-FC80D0AD8CE9}"/>
+    <cellStyle name="Normal 5 3" xfId="171" xr:uid="{BF019E75-FCB3-47C3-88E2-E8420D3EBAA0}"/>
+    <cellStyle name="Normal 5 4" xfId="172" xr:uid="{840A48D8-BBE6-437E-9DC7-1760B6754808}"/>
+    <cellStyle name="Normal 6" xfId="173" xr:uid="{9B7C8AB8-9806-4D30-BF4F-F844AD8C38C3}"/>
+    <cellStyle name="Normal 6 2" xfId="174" xr:uid="{BE47F9AE-99AF-45C8-8143-3F15DB722DF8}"/>
+    <cellStyle name="Normal 6 2 2" xfId="175" xr:uid="{94649937-4335-44E3-846B-F1E0AFFBEB8D}"/>
+    <cellStyle name="Normal 7" xfId="176" xr:uid="{D15EBA3D-DF07-4C7E-A7CD-F52FA16B3447}"/>
+    <cellStyle name="Normal 7 2" xfId="177" xr:uid="{CC694246-CF12-4FE9-9138-1D9C773E646E}"/>
+    <cellStyle name="Normal 7 2 2" xfId="178" xr:uid="{587387EA-C4F6-43ED-94E2-7FE194DBF1B5}"/>
+    <cellStyle name="Normal 7 2 3" xfId="179" xr:uid="{08774165-48E2-40F7-8F81-B1A5DE5512A5}"/>
+    <cellStyle name="Normal 7 3" xfId="180" xr:uid="{C2D6737F-26B0-40F5-8475-AC5B56027AF9}"/>
+    <cellStyle name="Normal 7 3 2" xfId="181" xr:uid="{B2C87768-EB9D-4D1F-A71B-C6E4DC23E274}"/>
+    <cellStyle name="Normal 7 3 3" xfId="182" xr:uid="{220B2FB5-5A59-4EB4-8CB6-3CA305F081F6}"/>
+    <cellStyle name="Normal 7 4" xfId="183" xr:uid="{721B16A0-FF51-419E-BE1D-8AFC27E2270E}"/>
+    <cellStyle name="Normal 7 5" xfId="184" xr:uid="{EE97706D-6588-4CC2-98CB-F19BDB100A5E}"/>
+    <cellStyle name="Normal 8" xfId="185" xr:uid="{338CB026-AB04-4A12-83F5-06D54D448B44}"/>
+    <cellStyle name="Normal 8 2" xfId="186" xr:uid="{D85BF6B0-9AA3-48BA-87DA-C15475BBE04D}"/>
+    <cellStyle name="Normal 8 2 2" xfId="187" xr:uid="{EFF0BF5C-395C-4606-9B8B-04C56210992F}"/>
+    <cellStyle name="Normal 8 2 3" xfId="188" xr:uid="{DEB13E0F-13CD-4F93-879E-31783269801B}"/>
+    <cellStyle name="Normal 8 3" xfId="189" xr:uid="{4ADAA56E-1036-4073-9A82-B2F9706FB217}"/>
+    <cellStyle name="Normal 8 3 2" xfId="190" xr:uid="{D83984CC-E451-496F-9895-65D4BB37E518}"/>
+    <cellStyle name="Normal 9" xfId="191" xr:uid="{793701A7-8D28-42C3-B890-73EFED806374}"/>
+    <cellStyle name="Normal 9 2" xfId="192" xr:uid="{3E582D53-ABCA-4CAB-80BC-B4A288608194}"/>
+    <cellStyle name="Normal 9 2 2" xfId="193" xr:uid="{AA1963EA-9A87-46EE-BAAD-09DBF2588D19}"/>
+    <cellStyle name="Normal 9 2 3" xfId="194" xr:uid="{FE49E57A-47D1-46D7-BB1D-AE5DC4342750}"/>
+    <cellStyle name="Normal 9 3" xfId="195" xr:uid="{42F53A55-05CB-435C-8567-3E9333A1C5C0}"/>
+    <cellStyle name="Note 2" xfId="196" xr:uid="{2E9A66CB-CA26-4B71-A1DB-E5854EDDBBC4}"/>
+    <cellStyle name="Note 3" xfId="197" xr:uid="{3BBB83BE-F32B-419F-A9C7-C18C16AD2EF5}"/>
+    <cellStyle name="Note 4" xfId="198" xr:uid="{3D99F797-CE2D-406E-8B77-123FA4ED8DD5}"/>
+    <cellStyle name="Note 5" xfId="199" xr:uid="{EC76D050-9990-4C86-BE7C-F1C59BB635B6}"/>
+    <cellStyle name="Note 6" xfId="200" xr:uid="{37B3F5DE-972C-4595-A89C-F6F03E8B9BDF}"/>
+    <cellStyle name="Notification" xfId="201" xr:uid="{35C8F0BB-2770-4963-BF23-F49444FF2BE3}"/>
+    <cellStyle name="Percent 2" xfId="202" xr:uid="{7DD09E8C-C2C0-4A08-ADBB-D3316161F1CA}"/>
+    <cellStyle name="Percent 2 2" xfId="203" xr:uid="{CF886FFF-7647-47F3-9971-547896E95325}"/>
+    <cellStyle name="Percent 2 2 2" xfId="204" xr:uid="{2DAE3409-A9F6-4D26-88B0-834EA893DD6A}"/>
+    <cellStyle name="Percent 3" xfId="205" xr:uid="{1388104E-0444-4F0D-B2B1-A16D0029766C}"/>
+    <cellStyle name="Percent 3 2" xfId="206" xr:uid="{750EC36E-1AF1-430A-974F-A59E73BFA5EF}"/>
+    <cellStyle name="Percent 3 2 2" xfId="207" xr:uid="{C1DE2851-8924-42D1-BAA4-75CB294872A5}"/>
+    <cellStyle name="Percent 3 3" xfId="208" xr:uid="{6E034C9C-DA6A-4EFF-BA06-744CAD6A5A37}"/>
+    <cellStyle name="Percent 4" xfId="209" xr:uid="{3E52E2EA-8A7D-44BF-9060-C2427C54CAE3}"/>
+    <cellStyle name="Pourcentage 2" xfId="210" xr:uid="{3A5274E3-6D5B-4C76-8035-0F55804B68AD}"/>
+    <cellStyle name="Pourcentage 2 2" xfId="211" xr:uid="{CCE7C477-1F92-468F-B778-41C5285D48F9}"/>
+    <cellStyle name="Pourcentage 2 2 2" xfId="247" xr:uid="{28A9CE28-A2BF-4532-9F85-B35FF2BA498E}"/>
+    <cellStyle name="Pourcentage 3" xfId="238" xr:uid="{82A08D9D-4832-481A-ABD8-93D3D21DB53D}"/>
+    <cellStyle name="Pourcentage 3 2" xfId="239" xr:uid="{6B45DEAF-752C-47C9-9C00-3E78934DA58C}"/>
     <cellStyle name="Вывод" xfId="1" builtinId="21"/>
+    <cellStyle name="Гиперссылка 2" xfId="212" xr:uid="{40A19919-B3D2-4654-BCE4-B67B5D87564B}"/>
+    <cellStyle name="Денежный 2" xfId="248" xr:uid="{183058FC-6E1C-4FEB-BED1-8FA56FD191D0}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="2" xr:uid="{8436E92C-B774-46C8-B4C4-A8F972A67876}"/>
+    <cellStyle name="Обычный 2 2" xfId="214" xr:uid="{E5561DDD-ACF8-4BAD-899F-8C00DF91489C}"/>
+    <cellStyle name="Обычный 2 3" xfId="213" xr:uid="{1A0ABB61-08BF-41B7-9E57-3BBB0CEEA8B7}"/>
+    <cellStyle name="Обычный 3" xfId="215" xr:uid="{0B43A6EA-9979-41C0-A430-81B8D5DF7065}"/>
+    <cellStyle name="Обычный 4" xfId="216" xr:uid="{BD8E3245-B55D-4DB6-A4E6-4D075CD67973}"/>
+    <cellStyle name="Обычный 5" xfId="217" xr:uid="{5FF75F1A-923C-4507-B920-EE60103D0407}"/>
+    <cellStyle name="Обычный 5 2" xfId="218" xr:uid="{C51D8C69-A886-403C-9FB7-F6BE4256415F}"/>
+    <cellStyle name="Обычный 5 3" xfId="219" xr:uid="{52BA9AC1-35B0-4484-9567-AF7B99A10E39}"/>
+    <cellStyle name="Обычный 6" xfId="220" xr:uid="{93F25311-C3C4-4845-8F98-60303D68375B}"/>
+    <cellStyle name="Обычный 7" xfId="4" xr:uid="{2D9B8703-A478-4C2C-868E-948B17C9F5BA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1085,10 +2607,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1400,46 +2918,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="51"/>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
-      <c r="L1" s="44"/>
+      <c r="L1" s="45"/>
     </row>
     <row r="2" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
-      <c r="L2" s="44"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="3" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="33"/>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
-      <c r="L3" s="44"/>
+      <c r="L3" s="45"/>
     </row>
     <row r="4" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="35"/>
@@ -1453,7 +2971,7 @@
       <c r="I4" s="33"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
-      <c r="L4" s="44"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="32"/>
@@ -1467,7 +2985,7 @@
       <c r="I5" s="31"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
-      <c r="L5" s="44"/>
+      <c r="L5" s="45"/>
     </row>
     <row r="6" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="32"/>
@@ -1481,7 +2999,7 @@
       <c r="I6" s="33"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
-      <c r="L6" s="44"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="32"/>
@@ -1495,7 +3013,7 @@
       <c r="I7" s="31"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
-      <c r="L7" s="44"/>
+      <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
@@ -1509,7 +3027,7 @@
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
-      <c r="L8" s="44"/>
+      <c r="L8" s="45"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
@@ -1523,49 +3041,49 @@
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
-      <c r="L9" s="44"/>
+      <c r="L9" s="45"/>
     </row>
     <row r="10" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
-      <c r="L10" s="44"/>
+      <c r="L10" s="45"/>
     </row>
     <row r="11" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="31"/>
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
-      <c r="L11" s="44"/>
+      <c r="L11" s="45"/>
     </row>
     <row r="12" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
       <c r="B12" s="33"/>
       <c r="C12" s="33"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="44"/>
+      <c r="L12" s="45"/>
     </row>
     <row r="13" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="32"/>
@@ -1579,7 +3097,7 @@
       <c r="I13" s="33"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
-      <c r="L13" s="44"/>
+      <c r="L13" s="45"/>
     </row>
     <row r="14" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="32"/>
@@ -1593,7 +3111,7 @@
       <c r="I14" s="33"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
-      <c r="L14" s="44"/>
+      <c r="L14" s="45"/>
     </row>
     <row r="15" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
@@ -1607,23 +3125,23 @@
       <c r="I15" s="33"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
-      <c r="L15" s="44"/>
+      <c r="L15" s="45"/>
     </row>
     <row r="16" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A16" s="32"/>
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
-      <c r="L16" s="44"/>
+      <c r="L16" s="45"/>
     </row>
     <row r="17" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="32"/>
@@ -1635,15 +3153,15 @@
       <c r="E17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
-      <c r="L17" s="44"/>
+      <c r="L17" s="45"/>
     </row>
     <row r="18" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="32"/>
@@ -1655,15 +3173,15 @@
       <c r="E18" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="49" t="s">
+      <c r="F18" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="44"/>
+      <c r="L18" s="45"/>
     </row>
     <row r="19" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
@@ -1687,7 +3205,7 @@
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="44"/>
+      <c r="L19" s="45"/>
     </row>
     <row r="20" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
@@ -1709,7 +3227,7 @@
       <c r="I20" s="13"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
-      <c r="L20" s="44"/>
+      <c r="L20" s="45"/>
     </row>
     <row r="21" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
@@ -1731,7 +3249,7 @@
       <c r="I21" s="18"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
-      <c r="L21" s="44"/>
+      <c r="L21" s="45"/>
     </row>
     <row r="22" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
@@ -1753,7 +3271,7 @@
       <c r="I22" s="13"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
-      <c r="L22" s="44"/>
+      <c r="L22" s="45"/>
     </row>
     <row r="23" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
@@ -1775,7 +3293,7 @@
       <c r="I23" s="18"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
-      <c r="L23" s="44"/>
+      <c r="L23" s="45"/>
     </row>
     <row r="24" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
@@ -1797,7 +3315,7 @@
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
-      <c r="L24" s="44"/>
+      <c r="L24" s="45"/>
     </row>
     <row r="25" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D25" s="11" t="s">
@@ -1814,7 +3332,7 @@
       <c r="I25" s="7">
         <v>10000</v>
       </c>
-      <c r="L25" s="44"/>
+      <c r="L25" s="45"/>
     </row>
     <row r="26" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
@@ -1823,7 +3341,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="L26" s="44"/>
+      <c r="L26" s="45"/>
     </row>
     <row r="27" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
@@ -1832,18 +3350,18 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="L27" s="44"/>
+      <c r="L27" s="45"/>
     </row>
     <row r="28" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="D28" s="50" t="s">
+      <c r="D28" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="L28" s="44"/>
+      <c r="L28" s="45"/>
     </row>
     <row r="29" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D29" s="2"/>
@@ -1852,7 +3370,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="L29" s="44"/>
+      <c r="L29" s="45"/>
     </row>
     <row r="30" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D30" s="2"/>
@@ -1861,18 +3379,18 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="L30" s="44"/>
+      <c r="L30" s="45"/>
     </row>
     <row r="31" spans="1:12" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="45"/>
+      <c r="E31" s="46"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="L31" s="44"/>
+      <c r="L31" s="45"/>
     </row>
     <row r="32" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D32" s="6" t="s">
@@ -1885,8 +3403,8 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="44"/>
-      <c r="L32" s="44"/>
+      <c r="J32" s="45"/>
+      <c r="L32" s="45"/>
     </row>
     <row r="33" spans="4:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D33" s="4" t="s">
@@ -1899,46 +3417,46 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="44"/>
-      <c r="L33" s="44"/>
+      <c r="J33" s="45"/>
+      <c r="L33" s="45"/>
     </row>
     <row r="34" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="J34" s="44"/>
-      <c r="L34" s="44"/>
+      <c r="J34" s="45"/>
+      <c r="L34" s="45"/>
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="J35" s="44"/>
-      <c r="L35" s="44"/>
+      <c r="J35" s="45"/>
+      <c r="L35" s="45"/>
     </row>
     <row r="36" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="J36" s="44"/>
-      <c r="L36" s="44"/>
+      <c r="J36" s="45"/>
+      <c r="L36" s="45"/>
     </row>
     <row r="37" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="J37" s="44"/>
-      <c r="L37" s="44"/>
+      <c r="J37" s="45"/>
+      <c r="L37" s="45"/>
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="J38" s="44"/>
+      <c r="J38" s="45"/>
     </row>
     <row r="39" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="J39" s="44"/>
+      <c r="J39" s="45"/>
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="J40" s="44"/>
+      <c r="J40" s="45"/>
     </row>
     <row r="41" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="J41" s="44"/>
+      <c r="J41" s="45"/>
     </row>
     <row r="42" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H42" s="44"/>
-      <c r="J42" s="44"/>
+      <c r="H42" s="45"/>
+      <c r="J42" s="45"/>
     </row>
     <row r="43" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H43" s="44"/>
+      <c r="H43" s="45"/>
     </row>
     <row r="44" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H44" s="44"/>
+      <c r="H44" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1967,7 +3485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E5CAF2-F9F1-4C07-82FF-78C8E1B3E25F}">
   <dimension ref="B3:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1977,21 +3495,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
     </row>
     <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="52"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="37"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="52"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="38"/>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
@@ -1999,10 +3517,10 @@
       <c r="J4" s="37"/>
     </row>
     <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B5" s="52"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="37"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="52"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="38"/>
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
@@ -2010,10 +3528,10 @@
       <c r="J5" s="37"/>
     </row>
     <row r="6" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B6" s="52"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="37"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="38"/>
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
@@ -2021,10 +3539,10 @@
       <c r="J6" s="37"/>
     </row>
     <row r="7" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B7" s="52"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="37"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="38"/>
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
@@ -2032,10 +3550,10 @@
       <c r="J7" s="37"/>
     </row>
     <row r="8" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B8" s="53"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="37"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="53"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
@@ -2043,10 +3561,10 @@
       <c r="J8" s="37"/>
     </row>
     <row r="9" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B9" s="53"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="37"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="53"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
@@ -2054,10 +3572,10 @@
       <c r="J9" s="37"/>
     </row>
     <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="54"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="37"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="53"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="54"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
@@ -2078,7 +3596,7 @@
     <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
-      <c r="D12" s="57"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="39"/>
       <c r="F12" s="40"/>
       <c r="G12" s="39"/>
@@ -2098,8 +3616,8 @@
       <c r="J13" s="39"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
       <c r="F14" s="41"/>
@@ -2109,8 +3627,8 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
       <c r="F15" s="41"/>
@@ -2219,21 +3737,21 @@
       <c r="J24" s="42"/>
     </row>
     <row r="27" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="55"/>
     </row>
     <row r="28" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B28" s="52"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="37"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="52"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="55"/>
       <c r="F28" s="38"/>
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
@@ -2241,10 +3759,10 @@
       <c r="J28" s="37"/>
     </row>
     <row r="29" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B29" s="52"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="37"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
       <c r="F29" s="38"/>
       <c r="G29" s="37"/>
       <c r="H29" s="37"/>
@@ -2252,10 +3770,10 @@
       <c r="J29" s="37"/>
     </row>
     <row r="30" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B30" s="52"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="37"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="56"/>
       <c r="F30" s="38"/>
       <c r="G30" s="37"/>
       <c r="H30" s="37"/>
@@ -2263,10 +3781,10 @@
       <c r="J30" s="37"/>
     </row>
     <row r="31" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B31" s="52"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="37"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="56"/>
       <c r="F31" s="37"/>
       <c r="G31" s="37"/>
       <c r="H31" s="37"/>
@@ -2274,10 +3792,10 @@
       <c r="J31" s="37"/>
     </row>
     <row r="32" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B32" s="53"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="37"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="53"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="54"/>
       <c r="F32" s="37"/>
       <c r="G32" s="37"/>
       <c r="H32" s="37"/>
@@ -2285,10 +3803,10 @@
       <c r="J32" s="37"/>
     </row>
     <row r="33" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B33" s="53"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="37"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="53"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="54"/>
       <c r="F33" s="37"/>
       <c r="G33" s="37"/>
       <c r="H33" s="37"/>
@@ -2329,8 +3847,8 @@
       <c r="J36" s="39"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
       <c r="D37" s="41"/>
       <c r="E37" s="41"/>
       <c r="F37" s="41"/>
@@ -2340,8 +3858,8 @@
       <c r="J37" s="41"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
       <c r="D38" s="41"/>
       <c r="E38" s="41"/>
       <c r="F38" s="41"/>
@@ -2451,6 +3969,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="B14:B15"/>
@@ -2463,17 +3990,371 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AAC96B-E29C-4873-AE39-AE2B342D43A7}">
+  <dimension ref="B4:AA13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B4" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="113"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="113"/>
+      <c r="S4" s="113"/>
+      <c r="T4" s="113"/>
+      <c r="U4" s="113"/>
+      <c r="V4" s="111"/>
+      <c r="W4" s="111"/>
+      <c r="X4" s="111"/>
+      <c r="Y4" s="111"/>
+      <c r="Z4" s="111"/>
+      <c r="AA4" s="111"/>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B5" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="100" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B6" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="94"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+    </row>
+    <row r="7" spans="2:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="95"/>
+      <c r="S7" s="61"/>
+      <c r="T7" s="61"/>
+      <c r="U7" s="61"/>
+    </row>
+    <row r="8" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="106" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="102"/>
+      <c r="M8" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="98"/>
+      <c r="S8" s="98"/>
+      <c r="T8" s="98"/>
+      <c r="U8" s="99"/>
+    </row>
+    <row r="9" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="105"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="102"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="102"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="101" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="102"/>
+      <c r="L9" s="103"/>
+      <c r="M9" s="108" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9" s="109"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="108" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="97" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" s="98"/>
+      <c r="U9" s="99"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B10" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="73">
+        <v>1</v>
+      </c>
+      <c r="E10" s="81">
+        <v>2</v>
+      </c>
+      <c r="F10" s="82">
+        <v>3</v>
+      </c>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="92"/>
+      <c r="M10" s="86">
+        <v>10</v>
+      </c>
+      <c r="N10" s="76">
+        <v>11</v>
+      </c>
+      <c r="O10" s="74"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="90"/>
+      <c r="T10" s="91"/>
+      <c r="U10" s="92"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B11" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="65"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67">
+        <v>4</v>
+      </c>
+      <c r="H11" s="77">
+        <v>5</v>
+      </c>
+      <c r="I11" s="84"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="67">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="77">
+        <v>13</v>
+      </c>
+      <c r="R11" s="84"/>
+      <c r="S11" s="67"/>
+      <c r="T11" s="89"/>
+      <c r="U11" s="66"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B12" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="65"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67">
+        <v>6</v>
+      </c>
+      <c r="H12" s="77">
+        <v>7</v>
+      </c>
+      <c r="I12" s="84"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="67">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="77">
+        <v>15</v>
+      </c>
+      <c r="R12" s="84"/>
+      <c r="S12" s="67"/>
+      <c r="T12" s="89"/>
+      <c r="U12" s="66"/>
+    </row>
+    <row r="13" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="68"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="70">
+        <v>8</v>
+      </c>
+      <c r="H13" s="78">
+        <v>9</v>
+      </c>
+      <c r="I13" s="85"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="88"/>
+      <c r="N13" s="78"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="70">
+        <v>16</v>
+      </c>
+      <c r="Q13" s="78">
+        <v>17</v>
+      </c>
+      <c r="R13" s="85"/>
+      <c r="S13" s="70"/>
+      <c r="T13" s="93"/>
+      <c r="U13" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="M8:U8"/>
+    <mergeCell ref="B4:U4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="D8:L8"/>
+  </mergeCells>
+  <phoneticPr fontId="47" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>